<commit_message>
get support test case created and purchase attemp log reviewed
</commit_message>
<xml_diff>
--- a/apps/features/redmine/payment management/add new event code/add_new_event-code.xlsx
+++ b/apps/features/redmine/payment management/add new event code/add_new_event-code.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\redmine\payment management\add new event code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4665D0-4A80-40D5-9D5F-E7C917D318EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0520A9-D2FB-4DCF-865D-97B34E6E6F59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -274,6 +274,9 @@
     <t>enter the same code in different cases 
 (e.g. ABC and abc)</t>
   </si>
+  <si>
+    <t>Pass</t>
+  </si>
 </sst>
 </file>
 
@@ -324,7 +327,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +356,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
         <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -499,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -569,6 +578,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -577,7 +589,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1400,8 +1412,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1418,15 +1430,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -1448,13 +1460,13 @@
       <c r="Z1" s="18"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -1649,7 +1661,9 @@
       <c r="E7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
@@ -1687,7 +1701,9 @@
       <c r="E8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="24"/>
       <c r="I8" s="24"/>
@@ -1725,7 +1741,9 @@
       <c r="E9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="G9" s="14"/>
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
@@ -1763,7 +1781,9 @@
       <c r="E10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="G10" s="14"/>
       <c r="H10" s="24"/>
       <c r="I10" s="24"/>
@@ -1801,7 +1821,7 @@
       <c r="E11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="15"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
@@ -1839,7 +1859,9 @@
       <c r="E12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="G12" s="15"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
@@ -1877,7 +1899,7 @@
       <c r="E13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="15"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
@@ -1915,7 +1937,7 @@
       <c r="E14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="15"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
@@ -1953,7 +1975,7 @@
       <c r="E15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="16"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
@@ -1991,7 +2013,7 @@
       <c r="E16" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="16"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
@@ -2029,7 +2051,7 @@
       <c r="E17" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="32"/>
       <c r="G17" s="16"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -2067,7 +2089,7 @@
       <c r="E18" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="16"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
@@ -2105,7 +2127,7 @@
       <c r="E19" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="16"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
@@ -2143,7 +2165,7 @@
       <c r="E20" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="16"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="16"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -2181,7 +2203,7 @@
       <c r="E21" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="32"/>
       <c r="G21" s="16"/>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -2219,7 +2241,9 @@
       <c r="E22" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="32" t="s">
+        <v>75</v>
+      </c>
       <c r="G22" s="16"/>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
@@ -2257,7 +2281,9 @@
       <c r="E23" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="16"/>
+      <c r="F23" s="32" t="s">
+        <v>75</v>
+      </c>
       <c r="G23" s="16"/>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
@@ -2295,7 +2321,9 @@
       <c r="E24" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="32" t="s">
+        <v>75</v>
+      </c>
       <c r="G24" s="16"/>
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
@@ -2324,7 +2352,7 @@
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="25" t="s">
         <v>71</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -2333,7 +2361,9 @@
       <c r="E25" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F25" s="16"/>
+      <c r="F25" s="32" t="s">
+        <v>75</v>
+      </c>
       <c r="G25" s="16"/>
       <c r="H25" s="18"/>
       <c r="I25" s="18"/>
@@ -29380,7 +29410,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F5:F8" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F5:F25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>